<commit_message>
commenting and minor optimizations
</commit_message>
<xml_diff>
--- a/summer2.xlsx
+++ b/summer2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ebf90761794f767e/Docs/Sem 6/Subjects/Mini Project/RookieCook/weather_module/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="224" documentId="8_{39624778-9EE1-45F0-88EC-A238BA68C2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37EBC1DD-BBD9-48CB-B069-CCAAB58573ED}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="8_{39624778-9EE1-45F0-88EC-A238BA68C2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24EDC028-81EA-4840-A659-8AEEE84E449C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="14880" xr2:uid="{1FA58EFA-933D-44A8-8461-C532784C456B}"/>
+    <workbookView minimized="1" xWindow="-21255" yWindow="2265" windowWidth="15900" windowHeight="9720" xr2:uid="{1FA58EFA-933D-44A8-8461-C532784C456B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>prefer_in_summer</t>
   </si>
@@ -343,10 +343,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -648,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44239FC-5065-43E0-9C95-781687D03FE1}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,7 +770,7 @@
         <v>68</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -782,7 +778,7 @@
         <v>83</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -790,7 +786,7 @@
         <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>80</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -798,7 +794,7 @@
         <v>67</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -806,7 +802,7 @@
         <v>66</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -814,7 +810,7 @@
         <v>65</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>81</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -822,7 +818,7 @@
         <v>64</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -830,7 +826,7 @@
         <v>63</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -838,7 +834,7 @@
         <v>62</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -846,16 +842,13 @@
         <v>27</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -1033,8 +1026,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B24">
-    <sortCondition ref="B24"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B23">
+    <sortCondition ref="B23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>